<commit_message>
finished everthing except table
</commit_message>
<xml_diff>
--- a/house_info.xlsx
+++ b/house_info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="145">
   <si>
     <t xml:space="preserve">QUESTION</t>
   </si>
@@ -356,7 +356,112 @@
     <t xml:space="preserve">Interior layout</t>
   </si>
   <si>
-    <t xml:space="preserve">Basement</t>
+    <t xml:space="preserve">Basement  separate entrance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">basement_rooms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">living/dining/kitchen/rec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,0,0,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">family/den/laundry/storage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,0,1,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bed/full bath/2-piece bath </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,1,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exterior brick=0/stone=1/vinyl=2/concrete=3/stucco=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exterior_finish </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Floor: living+dining+kitchen? (0 or 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interior1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">family room/den/office/laundry </t>
+  </si>
+  <si>
+    <t xml:space="preserve">storey_rooms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,0,0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">master bed/ average bed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ensuite/full/partial bathroom </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,0,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flooring hardwood=0/broadloom=1/laminate=2/ceramic=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interior1_floor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second Floor living+dining+kitchen? (0 or 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interior2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">loft/den/office/laundry </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,0,0,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,1,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hardwood=0/broadloom=1/laminate=2/ceramic=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interior2_floor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Third Floor loft/den/office/laundry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interior3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hardwood=0/broadloom=1/ceramic=2/laminate=3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interior upgrades potlight=0/crown mouldings=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interior_finishes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,1</t>
   </si>
 </sst>
 </file>
@@ -367,7 +472,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -406,6 +511,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -450,7 +560,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -483,6 +593,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,10 +618,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -521,10 +639,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="22.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="21.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="31.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="31.69"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="15.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="22.09"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="19" style="1" width="11.54"/>
   </cols>
@@ -989,6 +1107,191 @@
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>109</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0"/>
+      <c r="B46" s="0"/>
+      <c r="C46" s="0"/>
+      <c r="D46" s="0"/>
+    </row>
+    <row r="47" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added auto fill table
</commit_message>
<xml_diff>
--- a/house_info.xlsx
+++ b/house_info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="149">
   <si>
     <t xml:space="preserve">QUESTION</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">storey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
   </si>
   <si>
     <t xml:space="preserve">For Freehold: 
@@ -452,7 +455,16 @@
     <t xml:space="preserve">interior3</t>
   </si>
   <si>
-    <t xml:space="preserve">hardwood=0/broadloom=1/ceramic=2/laminate=3 </t>
+    <t xml:space="preserve">0,0,0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,1,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,1,2</t>
   </si>
   <si>
     <t xml:space="preserve">Interior upgrades potlight=0/crown mouldings=1</t>
@@ -518,12 +530,66 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF5CE"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8000"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF729FCF"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8F2A1"/>
+        <bgColor rgb="FFFFF5CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBBE33D"/>
+        <bgColor rgb="FFE8F2A1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5EB91E"/>
+        <bgColor rgb="FF468A1A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF468A1A"/>
+        <bgColor rgb="FF5EB91E"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -560,7 +626,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -569,8 +635,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -581,6 +655,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -589,7 +667,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -597,7 +695,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -610,6 +732,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF5EB91E"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF729FCF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFF5CE"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFE8F2A1"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FFBBE33D"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF8000"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF468A1A"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -620,15 +802,15 @@
   </sheetPr>
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E48" activeCellId="0" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="51.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.63"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="3" min="3" style="1" width="7.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="28.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="33.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.99"/>
@@ -662,7 +844,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -673,18 +855,18 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -695,7 +877,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -706,446 +888,446 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="1" t="n">
-        <v>2</v>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="C7" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>24</v>
+      <c r="A9" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="27.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>27</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>28</v>
+      <c r="A11" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
-        <v>30</v>
+      <c r="A12" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>32</v>
+      <c r="A13" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
-        <v>35</v>
+      <c r="A14" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
-        <v>38</v>
+      <c r="A15" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="3" t="s">
         <v>41</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="F15" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="4" t="s">
+      <c r="A16" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="B16" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="C16" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>46</v>
       </c>
+      <c r="B17" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="D17" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
-        <v>48</v>
+      <c r="A18" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>50</v>
+      <c r="A19" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>60</v>
+      <c r="A24" s="7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>61</v>
+      <c r="A25" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>64</v>
+      <c r="A26" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D26" s="5" t="s">
         <v>66</v>
       </c>
+      <c r="D26" s="8" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>67</v>
+      <c r="A27" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="6" t="s">
         <v>69</v>
       </c>
+      <c r="D27" s="9" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>70</v>
+      <c r="A28" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="11" t="n">
+        <v>1266480</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D29" s="7" t="n">
-        <v>1266480</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
     <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="D42" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="8" t="s">
-        <v>113</v>
+      <c r="A43" s="14" t="s">
+        <v>114</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="8" t="s">
-        <v>115</v>
+      <c r="A44" s="14" t="s">
+        <v>116</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1155,143 +1337,155 @@
       <c r="D46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B47" s="8" t="s">
+      <c r="A47" s="15" t="s">
         <v>118</v>
       </c>
+      <c r="B47" s="16" t="s">
+        <v>119</v>
+      </c>
       <c r="D47" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B48" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="53" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B53" s="8" t="s">
+      <c r="A53" s="18" t="s">
         <v>132</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>133</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="8" t="s">
-        <v>133</v>
+      <c r="A54" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="8" t="s">
-        <v>125</v>
+      <c r="A55" s="19" t="s">
+        <v>126</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="8" t="s">
-        <v>127</v>
+      <c r="A56" s="19" t="s">
+        <v>128</v>
       </c>
       <c r="D56" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B57" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="B57" s="9" t="s">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="8" t="s">
-        <v>141</v>
+      <c r="D61" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>143</v>
+      <c r="A62" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>147</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added comment city part
</commit_message>
<xml_diff>
--- a/house_info.xlsx
+++ b/house_info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="151">
   <si>
     <t xml:space="preserve">QUESTION</t>
   </si>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">district</t>
   </si>
   <si>
-    <t xml:space="preserve">?</t>
+    <t xml:space="preserve">Abbottsville Crossing</t>
   </si>
   <si>
     <t xml:space="preserve">Free=0/condo=1 </t>
@@ -67,13 +67,13 @@
     <t xml:space="preserve">type</t>
   </si>
   <si>
+    <t xml:space="preserve">Storey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storey</t>
+  </si>
+  <si>
     <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Storey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">storey</t>
   </si>
   <si>
     <t xml:space="preserve">For Freehold: 
@@ -86,6 +86,9 @@
     <t xml:space="preserve">.split(',') </t>
   </si>
   <si>
+    <t xml:space="preserve">irregular,interior,other residential lots</t>
+  </si>
+  <si>
     <t xml:space="preserve">rectangular,interior,other residential lots</t>
   </si>
   <si>
@@ -105,7 +108,7 @@
     <t xml:space="preserve">townhouse_location</t>
   </si>
   <si>
-    <t xml:space="preserve">interior</t>
+    <t xml:space="preserve">end</t>
   </si>
   <si>
     <t xml:space="preserve">street type
@@ -169,13 +172,16 @@
     <t xml:space="preserve">adverse_range</t>
   </si>
   <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nearby park/school </t>
   </si>
   <si>
     <t xml:space="preserve">facilities </t>
   </si>
   <si>
-    <t xml:space="preserve">Guinness Park</t>
+    <t xml:space="preserve">Abbottsville Trail, Bradley Commons Park</t>
   </si>
   <si>
     <t xml:space="preserve">electric underground=0/overhead=1 </t>
@@ -199,13 +205,13 @@
     <t xml:space="preserve">year_built</t>
   </si>
   <si>
-    <t xml:space="preserve">2021</t>
+    <t xml:space="preserve">2020</t>
   </si>
   <si>
     <t xml:space="preserve">sqft</t>
   </si>
   <si>
-    <t xml:space="preserve">1276</t>
+    <t xml:space="preserve">2400</t>
   </si>
   <si>
     <t xml:space="preserve">extra ownership checkbox
@@ -215,9 +221,6 @@
     <t xml:space="preserve">ownership_restriction_checkbox </t>
   </si>
   <si>
-    <t xml:space="preserve">y</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sales History</t>
   </si>
   <si>
@@ -227,7 +230,7 @@
     <t xml:space="preserve">geo_date</t>
   </si>
   <si>
-    <t xml:space="preserve">1997-03-07</t>
+    <t xml:space="preserve">2020-04-21</t>
   </si>
   <si>
     <t xml:space="preserve">geo name</t>
@@ -236,7 +239,7 @@
     <t xml:space="preserve">geo_name</t>
   </si>
   <si>
-    <t xml:space="preserve">KEDROSKY, KAREN ELIZABETH; KEDROSKY, ROBERT GREGORY;</t>
+    <t xml:space="preserve">SOGOOD INVESTMENTS INCORPORATED; </t>
   </si>
   <si>
     <t xml:space="preserve">geo price</t>
@@ -245,7 +248,7 @@
     <t xml:space="preserve">geo_price</t>
   </si>
   <si>
-    <t xml:space="preserve">263000</t>
+    <t xml:space="preserve">546027</t>
   </si>
   <si>
     <t xml:space="preserve">MLS Count? 0/1..</t>
@@ -263,12 +266,6 @@
     <t xml:space="preserve">mls_no</t>
   </si>
   <si>
-    <t xml:space="preserve">C5412187</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W4301258 </t>
-  </si>
-  <si>
     <t xml:space="preserve">///only takes 5 mls maximum</t>
   </si>
   <si>
@@ -278,13 +275,13 @@
     <t xml:space="preserve">mls_date</t>
   </si>
   <si>
-    <t xml:space="preserve">2021-11-09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021-10-25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-11-12</t>
+    <t xml:space="preserve">2021-09-21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-08-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-04-06</t>
   </si>
   <si>
     <t xml:space="preserve">2017-10-04</t>
@@ -296,13 +293,13 @@
     <t xml:space="preserve">listing_price</t>
   </si>
   <si>
-    <t xml:space="preserve">625000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3450000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1259700</t>
+    <t xml:space="preserve">995900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1049000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">499000</t>
   </si>
   <si>
     <t xml:space="preserve">249900</t>
@@ -314,13 +311,13 @@
     <t xml:space="preserve">sold_price</t>
   </si>
   <si>
-    <t xml:space="preserve">647000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2988000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ter</t>
+    <t xml:space="preserve">967000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">can</t>
+  </si>
+  <si>
+    <t xml:space="preserve">520000</t>
   </si>
   <si>
     <t xml:space="preserve">exp</t>
@@ -332,12 +329,12 @@
     <t xml:space="preserve">dom</t>
   </si>
   <si>
+    <t xml:space="preserve">49</t>
+  </si>
+  <si>
     <t xml:space="preserve">11</t>
   </si>
   <si>
-    <t xml:space="preserve">14</t>
-  </si>
-  <si>
     <t xml:space="preserve">92</t>
   </si>
   <si>
@@ -353,13 +350,16 @@
     <t xml:space="preserve">psa_date</t>
   </si>
   <si>
+    <t xml:space="preserve">2021-10-04</t>
+  </si>
+  <si>
     <t xml:space="preserve">PSA Buyer</t>
   </si>
   <si>
     <t xml:space="preserve">psa_buyer</t>
   </si>
   <si>
-    <t xml:space="preserve">Gwenning Nicolas B Poirier &amp; Katherine Mary Poirier</t>
+    <t xml:space="preserve">Zhibin Zhang</t>
   </si>
   <si>
     <t xml:space="preserve">PSA Seller</t>
@@ -368,7 +368,7 @@
     <t xml:space="preserve">psa_seller</t>
   </si>
   <si>
-    <t xml:space="preserve">Ashley Beland &amp; Jason Beland</t>
+    <t xml:space="preserve">Zhang Ruilin</t>
   </si>
   <si>
     <t xml:space="preserve">PSA Price</t>
@@ -377,7 +377,7 @@
     <t xml:space="preserve">psa_price</t>
   </si>
   <si>
-    <t xml:space="preserve">610000</t>
+    <t xml:space="preserve">780000</t>
   </si>
   <si>
     <t xml:space="preserve">Interior layout</t>
@@ -398,13 +398,13 @@
     <t xml:space="preserve">family/den/laundry/storage</t>
   </si>
   <si>
-    <t xml:space="preserve">1,0,1,0</t>
+    <t xml:space="preserve">0,0,0,1</t>
   </si>
   <si>
     <t xml:space="preserve">bed/full bath/2-piece bath </t>
   </si>
   <si>
-    <t xml:space="preserve">0,0,0</t>
+    <t xml:space="preserve">1,1,0</t>
   </si>
   <si>
     <t xml:space="preserve">Exterior brick=0/stone=1/vinyl=2/concrete=3/stucco=4</t>
@@ -428,42 +428,36 @@
     <t xml:space="preserve">storey_rooms</t>
   </si>
   <si>
+    <t xml:space="preserve">master bed/ average bed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ensuite/full/partial bathroom </t>
+  </si>
+  <si>
+    <t xml:space="preserve">flooring hardwood=0/broadloom=1/laminate=2/ceramic=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interior1_floor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second Floor living+dining+kitchen? (0 or 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interior2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">loft/den/office/laundry </t>
+  </si>
+  <si>
     <t xml:space="preserve">1,0,0,0</t>
   </si>
   <si>
-    <t xml:space="preserve">master bed/ average bed </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ensuite/full/partial bathroom </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,0,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">flooring hardwood=0/broadloom=1/laminate=2/ceramic=3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">interior1_floor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Second Floor living+dining+kitchen? (0 or 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">interior2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">loft/den/office/laundry </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,2</t>
-  </si>
-  <si>
     <t xml:space="preserve">0,1,0</t>
   </si>
   <si>
@@ -473,19 +467,13 @@
     <t xml:space="preserve">interior2_floor</t>
   </si>
   <si>
+    <t xml:space="preserve">Third Floor loft/den/office/laundry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interior3</t>
+  </si>
+  <si>
     <t xml:space="preserve">1,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Third Floor loft/den/office/laundry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">interior3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,1,0</t>
   </si>
   <si>
     <t xml:space="preserve">Interior upgrades potlight=0/crown mouldings=1 empty = None</t>
@@ -538,7 +526,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="7"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -658,7 +646,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -687,19 +675,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -930,8 +922,8 @@
   </sheetPr>
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D54" activeCellId="0" sqref="D54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -993,7 +985,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1004,7 +996,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -1012,18 +1004,18 @@
         <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="25.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1039,60 +1031,64 @@
       <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F7" s="0"/>
+      <c r="G7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>12</v>
@@ -1100,41 +1096,41 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="35.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>12</v>
@@ -1142,35 +1138,35 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>12</v>
@@ -1178,239 +1174,239 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="5" t="s">
         <v>69</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
-        <v>73</v>
+      <c r="A28" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="s">
         <v>76</v>
       </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="8" t="s">
+        <v>77</v>
+      </c>
       <c r="B29" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D29" s="8" t="n">
-        <v>1270103</v>
-      </c>
-      <c r="E29" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="F29" s="9" t="s">
+      <c r="D29" s="9" t="n">
+        <v>1262485</v>
+      </c>
+      <c r="E29" s="9" t="n">
+        <v>1255871</v>
+      </c>
+      <c r="F29" s="10" t="n">
+        <v>1232391</v>
+      </c>
+      <c r="G29" s="11" t="n">
+        <v>1081047</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G29" s="10" t="n">
-        <v>1081047</v>
-      </c>
-      <c r="I29" s="1" t="s">
+    </row>
+    <row r="30" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="s">
+      <c r="B30" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="I30" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="I30" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="s">
+      <c r="B31" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="I31" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="I31" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7" t="s">
+      <c r="B32" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="I32" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="I32" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7" t="s">
+      <c r="B33" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="D33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="I33" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="I33" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11" t="s">
+      <c r="B34" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="D34" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="11" t="s">
+      <c r="B35" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="11" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="12" t="s">
         <v>108</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1420,8 +1416,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="11" t="s">
+    <row r="37" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="12" t="s">
         <v>111</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -1431,8 +1427,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="11" t="s">
+    <row r="38" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="12" t="s">
         <v>114</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1443,12 +1439,12 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="13" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="12" t="s">
+    <row r="41" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="13" t="s">
         <v>118</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1458,8 +1454,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="13" t="s">
+    <row r="42" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="14" t="s">
         <v>120</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -1469,8 +1465,8 @@
         <v>121</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="13" t="s">
+    <row r="43" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="14" t="s">
         <v>122</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -1480,8 +1476,8 @@
         <v>123</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="13" t="s">
+    <row r="44" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="14" t="s">
         <v>124</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -1491,8 +1487,8 @@
         <v>125</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="14" t="s">
+    <row r="47" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="15" t="s">
         <v>126</v>
       </c>
       <c r="B47" s="5" t="s">
@@ -1502,142 +1498,142 @@
         <v>128</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="14" t="s">
+    <row r="48" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="15" t="s">
         <v>129</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>130</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="16" t="s">
         <v>131</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>132</v>
       </c>
       <c r="D49" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="16" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="15" t="s">
+      <c r="D50" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D50" s="1" t="s">
+    </row>
+    <row r="51" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="16" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="15" t="s">
+      <c r="D51" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="14" t="s">
+      <c r="D52" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B52" s="1" t="s">
+    </row>
+    <row r="53" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="B53" s="5" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>142</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="17" t="s">
+    <row r="54" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="D55" s="1" t="s">
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="18" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="56" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="D56" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="57" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="17" t="s">
+      <c r="D57" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B58" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="19" t="s">
+    <row r="59" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D59" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="19" t="s">
-        <v>136</v>
+    </row>
+    <row r="60" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="20" t="s">
+        <v>135</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="19" t="s">
-        <v>146</v>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="20" t="s">
+        <v>144</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="20" t="s">
-        <v>153</v>
+    <row r="62" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="21" t="s">
+        <v>149</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1646,53 +1642,48 @@
       <formula>house_info!$D$34="n"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31:D33">
+  <conditionalFormatting sqref="D58:D61">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>house_info!$D$28="0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D58:D61">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(house_info!$D$6 &lt;&gt; "3",house_info!$D$6 &lt;&gt; "2 1/2")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53:D56">
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>OR(house_info!$D$6="1",house_info!$D$6 &lt;&gt; "3"="1 1/2")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D41:D44">
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>OR(house_info!$D$14="2",house_info!$D$14 ="3")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>house_info!$D$4 &lt;&gt; "1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>house_info!$D$4 &lt;&gt; "0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
-    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>house_info!$D$6 = "1"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>house_info!$D$5 = "3"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>OR(house_info!$D$4&lt;&gt;"0",house_info!$D$5&lt;&gt;"2")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D30:D33">
-    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+  <conditionalFormatting sqref="D31:F33">
+    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>house_info!$D$28="0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30:F33">
+    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>house_info!$D$28 = "0"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>